<commit_message>
Update xls input and creative script
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/TestData_Advertiser.xlsx
+++ b/src/test/resources/Data/TestData_Advertiser.xlsx
@@ -9,20 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13320" windowHeight="5960" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="14" r:id="rId1"/>
     <sheet name="AddPermit" sheetId="11" r:id="rId2"/>
     <sheet name="AddMatchWithoutUmp" sheetId="12" r:id="rId3"/>
     <sheet name="Advertiser" sheetId="1" r:id="rId4"/>
+    <sheet name="Creative" sheetId="15" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="16" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="76">
   <si>
     <t>TC NO</t>
   </si>
@@ -93,45 +95,15 @@
     <t>Testcase_002</t>
   </si>
   <si>
-    <t>Add a New Match with same Home and Away team</t>
-  </si>
-  <si>
-    <t>Home Team and Away Team should not be same</t>
-  </si>
-  <si>
     <t>Testcase_003</t>
   </si>
   <si>
-    <t xml:space="preserve">Add a New Match  with same Away Team and Umpire Team </t>
-  </si>
-  <si>
-    <t>Away Team and Umpire Teams should not be same</t>
-  </si>
-  <si>
-    <t>Testcase_004</t>
-  </si>
-  <si>
-    <t>Home Team and Umpire Teams should not be same</t>
-  </si>
-  <si>
-    <t>Testcase_005</t>
-  </si>
-  <si>
-    <t>Testcase_006</t>
-  </si>
-  <si>
-    <t>Testcase_007</t>
-  </si>
-  <si>
     <t>Absolute</t>
   </si>
   <si>
     <t>Warriors</t>
   </si>
   <si>
-    <t xml:space="preserve">Add a New Match with same  Home Team and Umpire Team </t>
-  </si>
-  <si>
     <t>Alpha Lions</t>
   </si>
   <si>
@@ -192,9 +164,6 @@
     <t>03/03/2024</t>
   </si>
   <si>
-    <t>03/24/2024</t>
-  </si>
-  <si>
     <t>TC_004</t>
   </si>
   <si>
@@ -204,16 +173,85 @@
     <t>Email is required. Password is required.</t>
   </si>
   <si>
-    <t>Advertiser_Name</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Desc</t>
+    <t>name</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>Automation Advertiser</t>
+  </si>
+  <si>
+    <t>CreativeMode</t>
+  </si>
+  <si>
+    <t>CreativeType</t>
+  </si>
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <t>Automation Creative</t>
+  </si>
+  <si>
+    <t>AdSource</t>
+  </si>
+  <si>
+    <t>Edge Ad Source</t>
+  </si>
+  <si>
+    <t>Upload</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>1Image.jpg</t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>2Video.mp4</t>
+  </si>
+  <si>
+    <t>HTML5</t>
+  </si>
+  <si>
+    <t>300x250Banner.jpg</t>
+  </si>
+  <si>
+    <t>TC_005</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>Ogx.zip</t>
+  </si>
+  <si>
+    <t>TC_006</t>
+  </si>
+  <si>
+    <t>CreativeURL</t>
+  </si>
+  <si>
+    <t>TC_007</t>
+  </si>
+  <si>
+    <t>TC_008</t>
+  </si>
+  <si>
+    <t>Vast</t>
+  </si>
+  <si>
+    <t>https://dummyimage.com/400x300/00ff00/000</t>
+  </si>
+  <si>
+    <t>http://commondatastorage.googleapis.com/gtv-videos-bucket/sample/ForBiggerJoyrides.mp4</t>
+  </si>
+  <si>
+    <t>https://ytvastqa.appspot.com/static/sampletag/vast.xml</t>
   </si>
 </sst>
 </file>
@@ -381,7 +419,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -430,9 +468,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -448,6 +483,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -738,82 +775,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="C2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>37</v>
-      </c>
-      <c r="C1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>47</v>
       </c>
       <c r="D3">
         <v>123456</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>43</v>
+      <c r="A4" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>33</v>
       </c>
       <c r="D4">
         <v>123456</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>58</v>
+      <c r="A5" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -842,42 +879,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="17" t="s">
+      <c r="A1" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" thickBot="1">
-      <c r="A2" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>40</v>
+      <c r="A2" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>17</v>
       </c>
     </row>
@@ -967,7 +1004,7 @@
         <v>14</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>15</v>
@@ -979,10 +1016,10 @@
         <v>17</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="I2" s="13"/>
       <c r="J2" s="13"/>
@@ -1010,7 +1047,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>15</v>
@@ -1022,10 +1059,10 @@
         <v>17</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="I3" s="13"/>
       <c r="J3" s="13" t="s">
@@ -1049,13 +1086,13 @@
     </row>
     <row r="4" spans="1:19" ht="29.5" thickBot="1">
       <c r="A4" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>15</v>
@@ -1067,13 +1104,13 @@
         <v>17</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="J4" s="13"/>
       <c r="K4" s="13" t="s">
@@ -1099,158 +1136,292 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9" style="5"/>
-    <col min="2" max="2" width="25.54296875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="12" style="6" customWidth="1"/>
-    <col min="5" max="5" width="33.26953125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="9" style="5"/>
-    <col min="7" max="7" width="35.1796875" style="5" customWidth="1"/>
+    <col min="1" max="3" width="9" style="5"/>
+    <col min="4" max="4" width="19.90625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" ht="15" thickBot="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-    </row>
-    <row r="2" spans="1:13" ht="29.5" thickBot="1">
-      <c r="A2" s="9" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-    </row>
-    <row r="3" spans="1:13" ht="29.5" thickBot="1">
-      <c r="A3" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-    </row>
-    <row r="4" spans="1:13" ht="44" thickBot="1">
-      <c r="A4" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="16" t="s">
+      <c r="B1" s="21" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="44" thickBot="1">
-      <c r="A5" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="10" t="s">
+      <c r="C1" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="16" t="s">
+      <c r="D1" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="21" t="s">
         <v>29</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="6" max="6" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="21"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G8" r:id="rId1"/>
+    <hyperlink ref="G7" r:id="rId2"/>
+    <hyperlink ref="G9" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>